<commit_message>
Actualizado a la fecha
</commit_message>
<xml_diff>
--- a/DocumentacionProyecto/Backlog/MIHuerto-Bloomhood - Backlog 1.xlsx
+++ b/DocumentacionProyecto/Backlog/MIHuerto-Bloomhood - Backlog 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Universidad\Gestion del proceso de desarrollo de software\Parcial 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tareas\10 cuatrimestre\Gestión y Desarrollo de Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BC1608-A8C1-4027-95C9-B518D13A56FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5321C9D7-1D6A-4D65-88FF-448AFD165339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{EC2672B6-AC1B-4333-BBAB-2F07098D012C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{EC2672B6-AC1B-4333-BBAB-2F07098D012C}"/>
   </bookViews>
   <sheets>
     <sheet name="Información Sprints" sheetId="3" r:id="rId1"/>
@@ -732,7 +732,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -766,6 +766,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1116,17 +1117,17 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -1146,7 +1147,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -1166,7 +1167,7 @@
         <v>10.25</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1188,7 +1189,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1210,7 +1211,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -1232,7 +1233,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -1254,7 +1255,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -1276,7 +1277,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1301,22 +1302,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D17BD224-0269-4C39-86AB-7245540C981E}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
     <col min="2" max="2" width="37" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="32.5703125" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" customWidth="1"/>
+    <col min="6" max="7" width="13.5546875" customWidth="1"/>
+    <col min="8" max="8" width="32.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
       <c r="B1" s="6" t="s">
         <v>25</v>
@@ -1330,7 +1331,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="11" t="s">
         <v>20</v>
@@ -1344,7 +1345,7 @@
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="15"/>
       <c r="C3" s="16" t="s">
@@ -1356,7 +1357,7 @@
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="15"/>
       <c r="C4" s="16" t="s">
@@ -1368,7 +1369,7 @@
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="15"/>
       <c r="C5" s="16" t="s">
@@ -1380,7 +1381,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="15"/>
       <c r="C6" s="16"/>
@@ -1390,7 +1391,7 @@
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="18"/>
       <c r="C7" s="19"/>
@@ -1400,7 +1401,7 @@
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -1410,14 +1411,14 @@
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="22" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="23">
         <f>IF(SUM(D12:D25)=0,0,SUMIF(C12:C25,"Terminado",D12:D25)/SUM(D12:D25))</f>
-        <v>0.5</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -1425,7 +1426,7 @@
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -1435,7 +1436,7 @@
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
         <v>0</v>
       </c>
@@ -1461,7 +1462,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
         <v>32</v>
       </c>
@@ -1485,7 +1486,7 @@
       </c>
       <c r="H12" s="24"/>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>33</v>
       </c>
@@ -1509,7 +1510,7 @@
       </c>
       <c r="H13" s="24"/>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
         <v>34</v>
       </c>
@@ -1533,7 +1534,7 @@
       </c>
       <c r="H14" s="24"/>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="s">
         <v>35</v>
       </c>
@@ -1557,7 +1558,7 @@
       </c>
       <c r="H15" s="24"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
         <v>36</v>
       </c>
@@ -1581,7 +1582,7 @@
       </c>
       <c r="H16" s="24"/>
     </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
         <v>37</v>
       </c>
@@ -1605,7 +1606,7 @@
       </c>
       <c r="H17" s="24"/>
     </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="24" t="s">
         <v>38</v>
       </c>
@@ -1629,7 +1630,7 @@
       </c>
       <c r="H18" s="24"/>
     </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="24" t="s">
         <v>39</v>
       </c>
@@ -1653,7 +1654,7 @@
       </c>
       <c r="H19" s="24"/>
     </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
         <v>40</v>
       </c>
@@ -1661,7 +1662,7 @@
         <v>61</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D20" s="24">
         <v>2</v>
@@ -1677,7 +1678,7 @@
       </c>
       <c r="H20" s="24"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
         <v>41</v>
       </c>
@@ -1685,7 +1686,7 @@
         <v>56</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D21" s="24">
         <v>4</v>
@@ -1701,7 +1702,7 @@
       </c>
       <c r="H21" s="24"/>
     </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
         <v>42</v>
       </c>
@@ -1709,7 +1710,7 @@
         <v>58</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D22" s="24">
         <v>3</v>
@@ -1725,7 +1726,7 @@
       </c>
       <c r="H22" s="24"/>
     </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
         <v>43</v>
       </c>
@@ -1733,7 +1734,7 @@
         <v>60</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D23" s="24">
         <v>1</v>
@@ -1749,7 +1750,7 @@
       </c>
       <c r="H23" s="24"/>
     </row>
-    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
         <v>44</v>
       </c>
@@ -1773,7 +1774,7 @@
       </c>
       <c r="H24" s="24"/>
     </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
         <v>45</v>
       </c>
@@ -1825,24 +1826,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB88AC0-FCCC-4DB3-A288-45E96A91229C}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L43" sqref="L43"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="32.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" customWidth="1"/>
+    <col min="6" max="7" width="13.5546875" customWidth="1"/>
+    <col min="8" max="8" width="32.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
       <c r="B1" s="6" t="s">
         <v>25</v>
@@ -1856,7 +1857,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="11" t="s">
         <v>20</v>
@@ -1870,7 +1871,7 @@
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="15"/>
       <c r="C3" s="16" t="s">
@@ -1882,7 +1883,7 @@
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="15"/>
       <c r="C4" s="16" t="s">
@@ -1894,7 +1895,7 @@
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="15"/>
       <c r="C5" s="16" t="s">
@@ -1906,7 +1907,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="15"/>
       <c r="C6" s="16"/>
@@ -1916,7 +1917,7 @@
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="18"/>
       <c r="C7" s="19"/>
@@ -1926,7 +1927,7 @@
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -1936,14 +1937,14 @@
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="22" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="23">
         <f>IF(SUM(D12:D25)=0,0,SUMIF(C12:C25,"Terminado",D12:D25)/SUM(D12:D25))</f>
-        <v>8.5714285714285715E-2</v>
+        <v>0.62857142857142856</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -1951,7 +1952,7 @@
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -1961,7 +1962,7 @@
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
         <v>0</v>
       </c>
@@ -1987,7 +1988,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
         <v>65</v>
       </c>
@@ -1995,7 +1996,7 @@
         <v>79</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="D12" s="24">
         <v>2</v>
@@ -2011,7 +2012,7 @@
       </c>
       <c r="H12" s="24"/>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>66</v>
       </c>
@@ -2019,7 +2020,7 @@
         <v>80</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="D13" s="24">
         <v>3</v>
@@ -2035,7 +2036,7 @@
       </c>
       <c r="H13" s="24"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
         <v>67</v>
       </c>
@@ -2059,7 +2060,7 @@
       </c>
       <c r="H14" s="24"/>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="s">
         <v>68</v>
       </c>
@@ -2083,7 +2084,7 @@
       </c>
       <c r="H15" s="24"/>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
         <v>69</v>
       </c>
@@ -2107,7 +2108,7 @@
       </c>
       <c r="H16" s="24"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
         <v>70</v>
       </c>
@@ -2115,7 +2116,7 @@
         <v>85</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D17" s="24">
         <v>2</v>
@@ -2131,7 +2132,7 @@
       </c>
       <c r="H17" s="24"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="24" t="s">
         <v>71</v>
       </c>
@@ -2139,7 +2140,7 @@
         <v>86</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D18" s="24">
         <v>4</v>
@@ -2155,7 +2156,7 @@
       </c>
       <c r="H18" s="24"/>
     </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="24" t="s">
         <v>72</v>
       </c>
@@ -2163,7 +2164,7 @@
         <v>87</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D19" s="24">
         <v>3</v>
@@ -2179,7 +2180,7 @@
       </c>
       <c r="H19" s="24"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
         <v>73</v>
       </c>
@@ -2187,7 +2188,7 @@
         <v>88</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D20" s="24">
         <v>2</v>
@@ -2203,7 +2204,7 @@
       </c>
       <c r="H20" s="24"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
         <v>74</v>
       </c>
@@ -2211,7 +2212,7 @@
         <v>90</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D21" s="24">
         <v>3</v>
@@ -2227,7 +2228,7 @@
       </c>
       <c r="H21" s="24"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
         <v>75</v>
       </c>
@@ -2235,7 +2236,7 @@
         <v>89</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="D22" s="24">
         <v>5</v>
@@ -2251,7 +2252,7 @@
       </c>
       <c r="H22" s="24"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
         <v>76</v>
       </c>
@@ -2259,7 +2260,7 @@
         <v>91</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="D23" s="24">
         <v>3</v>
@@ -2275,7 +2276,7 @@
       </c>
       <c r="H23" s="24"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
         <v>77</v>
       </c>
@@ -2283,7 +2284,7 @@
         <v>92</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="D24" s="24">
         <v>2</v>
@@ -2299,7 +2300,7 @@
       </c>
       <c r="H24" s="24"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
         <v>78</v>
       </c>
@@ -2322,6 +2323,9 @@
         <v>48</v>
       </c>
       <c r="H25" s="24"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D26" s="27"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2354,21 +2358,21 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="32.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" customWidth="1"/>
+    <col min="6" max="7" width="13.5546875" customWidth="1"/>
+    <col min="8" max="8" width="32.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
       <c r="B1" s="6" t="s">
         <v>25</v>
@@ -2382,7 +2386,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="11" t="s">
         <v>20</v>
@@ -2396,7 +2400,7 @@
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="15"/>
       <c r="C3" s="16" t="s">
@@ -2408,7 +2412,7 @@
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="15"/>
       <c r="C4" s="16" t="s">
@@ -2420,7 +2424,7 @@
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="15"/>
       <c r="C5" s="16" t="s">
@@ -2432,7 +2436,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="15"/>
       <c r="C6" s="16"/>
@@ -2442,7 +2446,7 @@
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="18"/>
       <c r="C7" s="19"/>
@@ -2452,7 +2456,7 @@
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -2462,14 +2466,14 @@
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="22" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="23">
         <f>IF(SUM(D12:D35)=0,0,SUMIF(C12:C35,"Terminado",D12:D35)/SUM(D12:D35))</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.45</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -2477,7 +2481,7 @@
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -2487,7 +2491,7 @@
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
         <v>0</v>
       </c>
@@ -2513,7 +2517,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
         <v>94</v>
       </c>
@@ -2537,7 +2541,7 @@
       </c>
       <c r="H12" s="24"/>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>95</v>
       </c>
@@ -2561,7 +2565,7 @@
       </c>
       <c r="H13" s="24"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
         <v>96</v>
       </c>
@@ -2585,7 +2589,7 @@
       </c>
       <c r="H14" s="24"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="s">
         <v>97</v>
       </c>
@@ -2593,7 +2597,7 @@
         <v>120</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D15" s="24">
         <v>2</v>
@@ -2609,7 +2613,7 @@
       </c>
       <c r="H15" s="24"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
         <v>98</v>
       </c>
@@ -2617,7 +2621,7 @@
         <v>121</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D16" s="24">
         <v>3</v>
@@ -2633,7 +2637,7 @@
       </c>
       <c r="H16" s="24"/>
     </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
         <v>99</v>
       </c>
@@ -2641,7 +2645,7 @@
         <v>122</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D17" s="24">
         <v>3</v>
@@ -2657,7 +2661,7 @@
       </c>
       <c r="H17" s="24"/>
     </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="24" t="s">
         <v>100</v>
       </c>
@@ -2665,7 +2669,7 @@
         <v>123</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D18" s="24">
         <v>3</v>
@@ -2681,7 +2685,7 @@
       </c>
       <c r="H18" s="24"/>
     </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="24" t="s">
         <v>101</v>
       </c>
@@ -2689,7 +2693,7 @@
         <v>124</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D19" s="24">
         <v>1</v>
@@ -2705,7 +2709,7 @@
       </c>
       <c r="H19" s="24"/>
     </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
         <v>102</v>
       </c>
@@ -2713,7 +2717,7 @@
         <v>125</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D20" s="24">
         <v>2</v>
@@ -2729,7 +2733,7 @@
       </c>
       <c r="H20" s="24"/>
     </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
         <v>103</v>
       </c>
@@ -2737,7 +2741,7 @@
         <v>126</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D21" s="24">
         <v>1</v>
@@ -2753,7 +2757,7 @@
       </c>
       <c r="H21" s="24"/>
     </row>
-    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
         <v>104</v>
       </c>
@@ -2777,7 +2781,7 @@
       </c>
       <c r="H22" s="24"/>
     </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
         <v>105</v>
       </c>
@@ -2785,7 +2789,7 @@
         <v>129</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D23" s="24">
         <v>2</v>
@@ -2801,7 +2805,7 @@
       </c>
       <c r="H23" s="24"/>
     </row>
-    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
         <v>106</v>
       </c>
@@ -2809,7 +2813,7 @@
         <v>130</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D24" s="24">
         <v>3</v>
@@ -2825,7 +2829,7 @@
       </c>
       <c r="H24" s="24"/>
     </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
         <v>107</v>
       </c>
@@ -2833,7 +2837,7 @@
         <v>131</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D25" s="24">
         <v>2</v>
@@ -2849,7 +2853,7 @@
       </c>
       <c r="H25" s="24"/>
     </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="24" t="s">
         <v>108</v>
       </c>
@@ -2857,7 +2861,7 @@
         <v>134</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="D26" s="24">
         <v>4</v>
@@ -2873,7 +2877,7 @@
       </c>
       <c r="H26" s="24"/>
     </row>
-    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
         <v>111</v>
       </c>
@@ -2881,7 +2885,7 @@
         <v>135</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="D27" s="24">
         <v>3</v>
@@ -2897,7 +2901,7 @@
       </c>
       <c r="H27" s="24"/>
     </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="24" t="s">
         <v>109</v>
       </c>
@@ -2905,7 +2909,7 @@
         <v>132</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="D28" s="24">
         <v>4</v>
@@ -2921,7 +2925,7 @@
       </c>
       <c r="H28" s="24"/>
     </row>
-    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="24" t="s">
         <v>110</v>
       </c>
@@ -2929,7 +2933,7 @@
         <v>133</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="D29" s="24">
         <v>3</v>
@@ -2945,7 +2949,7 @@
       </c>
       <c r="H29" s="24"/>
     </row>
-    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="24" t="s">
         <v>111</v>
       </c>
@@ -2953,7 +2957,7 @@
         <v>136</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="D30" s="24">
         <v>3</v>
@@ -2969,7 +2973,7 @@
       </c>
       <c r="H30" s="24"/>
     </row>
-    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="24" t="s">
         <v>112</v>
       </c>
@@ -2977,7 +2981,7 @@
         <v>137</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="D31" s="24">
         <v>3</v>
@@ -2993,7 +2997,7 @@
       </c>
       <c r="H31" s="24"/>
     </row>
-    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
         <v>113</v>
       </c>
@@ -3017,7 +3021,7 @@
       </c>
       <c r="H32" s="24"/>
     </row>
-    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="24" t="s">
         <v>114</v>
       </c>
@@ -3041,7 +3045,7 @@
       </c>
       <c r="H33" s="24"/>
     </row>
-    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
         <v>115</v>
       </c>
@@ -3065,7 +3069,7 @@
       </c>
       <c r="H34" s="24"/>
     </row>
-    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="24" t="s">
         <v>116</v>
       </c>
@@ -3103,18 +3107,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ReferenceId xmlns="a99dccc5-c3d6-4dee-b644-ad212f720ad9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D5C667E35EEA3948952157D5415021FC" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="34e18f3a9b3dbeee59763d3d4cb6abdb">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="213b2d84-3d9b-4b3f-804d-aac06d647ac8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f592687f4d80cd68537ad7211d22c13a" ns2:_="">
-    <xsd:import namespace="213b2d84-3d9b-4b3f-804d-aac06d647ac8"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100995E34F7C80F51488DBBAB02B8D6FEC8" ma:contentTypeVersion="8" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="7f80b59a505a7e396ed17abc7d388295">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a99dccc5-c3d6-4dee-b644-ad212f720ad9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="842a9985cbe252c85ebf65000f7fec8a" ns2:_="">
+    <xsd:import namespace="a99dccc5-c3d6-4dee-b644-ad212f720ad9"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -3125,6 +3128,10 @@
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -3132,7 +3139,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="213b2d84-3d9b-4b3f-804d-aac06d647ac8" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a99dccc5-c3d6-4dee-b644-ad212f720ad9" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="ReferenceId" ma:index="8" nillable="true" ma:displayName="ReferenceId" ma:indexed="true" ma:internalName="ReferenceId">
@@ -3153,6 +3160,26 @@
     <xsd:element name="MediaServiceSearchProperties" ma:index="11" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="13" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="14" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="15" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -3256,29 +3283,33 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ReferenceId xmlns="213b2d84-3d9b-4b3f-804d-aac06d647ac8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A0F4325-AF1A-42BB-B7E4-A8F1B1AA6EA3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4CB366A-4C18-458D-BA00-5CE9F81A5D3C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="213b2d84-3d9b-4b3f-804d-aac06d647ac8"/>
+    <ds:schemaRef ds:uri="a99dccc5-c3d6-4dee-b644-ad212f720ad9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D1B80D0-50CA-4D32-9889-9DCA80664017}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81FE4637-1A4E-4B87-9A02-8505A6470615}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="213b2d84-3d9b-4b3f-804d-aac06d647ac8"/>
+    <ds:schemaRef ds:uri="a99dccc5-c3d6-4dee-b644-ad212f720ad9"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -3290,11 +3321,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4CB366A-4C18-458D-BA00-5CE9F81A5D3C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A0F4325-AF1A-42BB-B7E4-A8F1B1AA6EA3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="213b2d84-3d9b-4b3f-804d-aac06d647ac8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>